<commit_message>
updated codes to calc 95% ci
</commit_message>
<xml_diff>
--- a/ISMS_Birth_Prevalence_Pooled_Estimate_TEMPLATE_2023.07.27_CB_archived.xlsx
+++ b/ISMS_Birth_Prevalence_Pooled_Estimate_TEMPLATE_2023.07.27_CB_archived.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinzhao/DS_Projects/automate-pooled-epi-estimation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9FB5EB-3938-3A40-AB51-D2EA6B3B703D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5952724-5A60-2646-ADC2-A6FF39DA4EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="37340" windowHeight="21100" activeTab="1" xr2:uid="{D7FAB0B9-2CD3-41D2-B0DC-ADFFCD4F0375}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{D7FAB0B9-2CD3-41D2-B0DC-ADFFCD4F0375}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="8" r:id="rId1"/>
@@ -2727,7 +2727,7 @@
         <v>0.99999499998749986</v>
       </c>
       <c r="E15" s="67">
-        <f t="shared" ref="D15:K15" si="10">100000*SQRT((E8*(1-E8))/E7)</f>
+        <f t="shared" ref="E15:K15" si="10">100000*SQRT((E8*(1-E8))/E7)</f>
         <v>0.70710324564380278</v>
       </c>
       <c r="F15" s="67">
@@ -2821,7 +2821,7 @@
         <v>1.8181818181818181E-2</v>
       </c>
       <c r="E17" s="15">
-        <f t="shared" ref="D17:K17" si="13">E9*E16</f>
+        <f t="shared" ref="E17:K17" si="13">E9*E16</f>
         <v>3.6363636363636362E-2</v>
       </c>
       <c r="F17" s="15">
@@ -3842,8 +3842,8 @@
   </sheetPr>
   <dimension ref="B2:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="106" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
created functions to estimate pooled prev
</commit_message>
<xml_diff>
--- a/ISMS_Birth_Prevalence_Pooled_Estimate_TEMPLATE_2023.07.27_CB_archived.xlsx
+++ b/ISMS_Birth_Prevalence_Pooled_Estimate_TEMPLATE_2023.07.27_CB_archived.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinzhao/DS_Projects/automate-pooled-epi-estimation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5952724-5A60-2646-ADC2-A6FF39DA4EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4E86BE-3B97-5E43-A7BA-DD7BD6AFFE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{D7FAB0B9-2CD3-41D2-B0DC-ADFFCD4F0375}"/>
   </bookViews>
@@ -3842,8 +3842,8 @@
   </sheetPr>
   <dimension ref="B2:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="106" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6711,26 +6711,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e34e3d43-a237-43ab-a7a6-573be7bf6622">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7652fdb5-7de5-4fe4-8faa-42c0d4a41c0a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F29972C995E494E853D6F7C6814115F" ma:contentTypeVersion="12" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="538331fc669173c4e7338fbcbb8cddc3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e34e3d43-a237-43ab-a7a6-573be7bf6622" xmlns:ns3="7652fdb5-7de5-4fe4-8faa-42c0d4a41c0a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74988d3b0b135cc94c1631b9891d0865" ns2:_="" ns3:_="">
     <xsd:import namespace="e34e3d43-a237-43ab-a7a6-573be7bf6622"/>
@@ -6931,10 +6911,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e34e3d43-a237-43ab-a7a6-573be7bf6622">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7652fdb5-7de5-4fe4-8faa-42c0d4a41c0a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{300DC9C1-369E-4FB3-B297-F73EAFAEF446}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A88AE369-7167-4AAC-9F0B-AB168D28D693}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e34e3d43-a237-43ab-a7a6-573be7bf6622"/>
+    <ds:schemaRef ds:uri="7652fdb5-7de5-4fe4-8faa-42c0d4a41c0a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6957,20 +6968,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A88AE369-7167-4AAC-9F0B-AB168D28D693}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{300DC9C1-369E-4FB3-B297-F73EAFAEF446}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e34e3d43-a237-43ab-a7a6-573be7bf6622"/>
-    <ds:schemaRef ds:uri="7652fdb5-7de5-4fe4-8faa-42c0d4a41c0a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added cli tool codes
</commit_message>
<xml_diff>
--- a/ISMS_Birth_Prevalence_Pooled_Estimate_TEMPLATE_2023.07.27_CB_archived.xlsx
+++ b/ISMS_Birth_Prevalence_Pooled_Estimate_TEMPLATE_2023.07.27_CB_archived.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinzhao/DS_Projects/automate-pooled-epi-estimation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4E86BE-3B97-5E43-A7BA-DD7BD6AFFE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FA153F-CA14-5044-BE56-6F3D79FB3FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{D7FAB0B9-2CD3-41D2-B0DC-ADFFCD4F0375}"/>
   </bookViews>
@@ -3842,8 +3842,8 @@
   </sheetPr>
   <dimension ref="B2:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47:E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>